<commit_message>
info: ppp.py now prints in proper format, minor bug fixes
</commit_message>
<xml_diff>
--- a/data/branch.xlsx
+++ b/data/branch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Surojit Mondal\Desktop\sbi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34A58AF-6FAA-45C6-A05B-A18E0F66E723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE85129-8CA5-48CE-A337-2546D6B5C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="293">
+  <si>
+    <t>BRANCH_NAME</t>
+  </si>
+  <si>
+    <t>IFSC_CODE</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
   <si>
     <t>Agartala</t>
   </si>
@@ -172,6 +187,153 @@
     <t>Hubli</t>
   </si>
   <si>
+    <t>Indore Main</t>
+  </si>
+  <si>
+    <t>Itanagar</t>
+  </si>
+  <si>
+    <t>Jabalpur</t>
+  </si>
+  <si>
+    <t>Jaipur Main</t>
+  </si>
+  <si>
+    <t>Jammu</t>
+  </si>
+  <si>
+    <t>Jamshedpur</t>
+  </si>
+  <si>
+    <t>Jodhpur</t>
+  </si>
+  <si>
+    <t>Kanpur</t>
+  </si>
+  <si>
+    <t>Kochi</t>
+  </si>
+  <si>
+    <t>Kolkata Main</t>
+  </si>
+  <si>
+    <t>Lucknow</t>
+  </si>
+  <si>
+    <t>Ludhiana</t>
+  </si>
+  <si>
+    <t>Madurai</t>
+  </si>
+  <si>
+    <t>Mumbai Main</t>
+  </si>
+  <si>
+    <t>Mysore</t>
+  </si>
+  <si>
+    <t>Nagaur</t>
+  </si>
+  <si>
+    <t>Nagpur</t>
+  </si>
+  <si>
+    <t>Nainital</t>
+  </si>
+  <si>
+    <t>Nashik</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>Ooty</t>
+  </si>
+  <si>
+    <t>Panaji</t>
+  </si>
+  <si>
+    <t>Patiala</t>
+  </si>
+  <si>
+    <t>Patna</t>
+  </si>
+  <si>
+    <t>Pondicherry</t>
+  </si>
+  <si>
+    <t>Port Blair</t>
+  </si>
+  <si>
+    <t>Pune Main</t>
+  </si>
+  <si>
+    <t>Raipur</t>
+  </si>
+  <si>
+    <t>Rajkot</t>
+  </si>
+  <si>
+    <t>Ranchi</t>
+  </si>
+  <si>
+    <t>Rohtak</t>
+  </si>
+  <si>
+    <t>Rourkela</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Shillong</t>
+  </si>
+  <si>
+    <t>Shimla</t>
+  </si>
+  <si>
+    <t>Siliguri</t>
+  </si>
+  <si>
+    <t>Srinagar</t>
+  </si>
+  <si>
+    <t>Surat</t>
+  </si>
+  <si>
+    <t>Thane</t>
+  </si>
+  <si>
+    <t>Thrissur</t>
+  </si>
+  <si>
+    <t>Tirupati</t>
+  </si>
+  <si>
+    <t>Trichy</t>
+  </si>
+  <si>
+    <t>Udaipur</t>
+  </si>
+  <si>
+    <t>Ujjain</t>
+  </si>
+  <si>
+    <t>Vadodara</t>
+  </si>
+  <si>
+    <t>Varanasi</t>
+  </si>
+  <si>
+    <t>Vellore</t>
+  </si>
+  <si>
+    <t>Vijayawada</t>
+  </si>
+  <si>
+    <t>Visakhapatnam</t>
+  </si>
+  <si>
     <t>SBIN0000001</t>
   </si>
   <si>
@@ -235,6 +397,9 @@
     <t>SBIN0000021</t>
   </si>
   <si>
+    <t>SBIN0000336</t>
+  </si>
+  <si>
     <t>SBIN0000023</t>
   </si>
   <si>
@@ -319,6 +484,318 @@
     <t>SBIN0000050</t>
   </si>
   <si>
+    <t>SBIN0000022</t>
+  </si>
+  <si>
+    <t>SBIN0000051</t>
+  </si>
+  <si>
+    <t>SBIN0000052</t>
+  </si>
+  <si>
+    <t>SBIN0000053</t>
+  </si>
+  <si>
+    <t>SBIN0000054</t>
+  </si>
+  <si>
+    <t>MG Road, Agartala</t>
+  </si>
+  <si>
+    <t>Ashram Road, Ahmedabad</t>
+  </si>
+  <si>
+    <t>Station Road, Akbarpur</t>
+  </si>
+  <si>
+    <t>Civil Lines, Aligarh</t>
+  </si>
+  <si>
+    <t>Alipore Road, Kolkata</t>
+  </si>
+  <si>
+    <t>MG Marg, Allahabad</t>
+  </si>
+  <si>
+    <t>Near Clock Tower, Alwar</t>
+  </si>
+  <si>
+    <t>Main Road, Amravati</t>
+  </si>
+  <si>
+    <t>Golden Temple Road, Amritsar</t>
+  </si>
+  <si>
+    <t>GT Road, Asansol</t>
+  </si>
+  <si>
+    <t>Samarth Nagar, Aurangabad</t>
+  </si>
+  <si>
+    <t>Chandipur Road, Balasore</t>
+  </si>
+  <si>
+    <t>MG Road, Bangalore</t>
+  </si>
+  <si>
+    <t>Civil Lines, Bareilly</t>
+  </si>
+  <si>
+    <t>Gandhi Nagar, Berhampur</t>
+  </si>
+  <si>
+    <t>JLN Road, Bhagalpur</t>
+  </si>
+  <si>
+    <t>Waghawadi Road, Bhavnagar</t>
+  </si>
+  <si>
+    <t>Nehru Nagar, Bhilai</t>
+  </si>
+  <si>
+    <t>TT Nagar, Bhopal</t>
+  </si>
+  <si>
+    <t>Janpath, Bhubaneswar</t>
+  </si>
+  <si>
+    <t>Station Road, Bhuj</t>
+  </si>
+  <si>
+    <t>Link Road, Bilaspur</t>
+  </si>
+  <si>
+    <t>Sector 4, Bokaro</t>
+  </si>
+  <si>
+    <t>G T Road, Burdwan</t>
+  </si>
+  <si>
+    <t>Mavoor Road, Calicut</t>
+  </si>
+  <si>
+    <t>Sector 17, Chandigarh</t>
+  </si>
+  <si>
+    <t>Anna Salai, Chennai</t>
+  </si>
+  <si>
+    <t>Gandhipuram, Coimbatore</t>
+  </si>
+  <si>
+    <t>Buxi Bazar, Cuttack</t>
+  </si>
+  <si>
+    <t>Rajpur Road, Dehradun</t>
+  </si>
+  <si>
+    <t>Bank More, Dhanbad</t>
+  </si>
+  <si>
+    <t>H S Road, Dibrugarh</t>
+  </si>
+  <si>
+    <t>Benachity, Durgapur</t>
+  </si>
+  <si>
+    <t>Marine Drive, Ernakulam</t>
+  </si>
+  <si>
+    <t>Perundurai Road, Erode</t>
+  </si>
+  <si>
+    <t>Sector 15, Faridabad</t>
+  </si>
+  <si>
+    <t>Mall Road, Ferozepur</t>
+  </si>
+  <si>
+    <t>Infocity, Gandhinagar</t>
+  </si>
+  <si>
+    <t>GB Road, Gaya</t>
+  </si>
+  <si>
+    <t>GT Road, Ghaziabad</t>
+  </si>
+  <si>
+    <t>Bank Road, Gorakhpur</t>
+  </si>
+  <si>
+    <t>Arundelpet, Guntur</t>
+  </si>
+  <si>
+    <t>MG Road, Gurgaon</t>
+  </si>
+  <si>
+    <t>Panbazar, Guwahati</t>
+  </si>
+  <si>
+    <t>Lashkar, Gwalior</t>
+  </si>
+  <si>
+    <t>Nainital Road, Haldwani</t>
+  </si>
+  <si>
+    <t>Station Road, Hardoi</t>
+  </si>
+  <si>
+    <t>Near Bus Stand, Hissar</t>
+  </si>
+  <si>
+    <t>Dobson Road, Howrah</t>
+  </si>
+  <si>
+    <t>Lamington Road, Hubli</t>
+  </si>
+  <si>
+    <t>MG Road, Indore</t>
+  </si>
+  <si>
+    <t>Ganga Market, Itanagar</t>
+  </si>
+  <si>
+    <t>Napier Town, Jabalpur</t>
+  </si>
+  <si>
+    <t>MI Road, Jaipur</t>
+  </si>
+  <si>
+    <t>Residency Road, Jammu</t>
+  </si>
+  <si>
+    <t>Bistupur, Jamshedpur</t>
+  </si>
+  <si>
+    <t>Clock Tower, Jodhpur</t>
+  </si>
+  <si>
+    <t>Mall Road, Kanpur</t>
+  </si>
+  <si>
+    <t>MG Road, Kochi</t>
+  </si>
+  <si>
+    <t>Dalhousie Square, Kolkata</t>
+  </si>
+  <si>
+    <t>Hazratganj, Lucknow</t>
+  </si>
+  <si>
+    <t>Ferozepur Road, Ludhiana</t>
+  </si>
+  <si>
+    <t>West Veli Street, Madurai</t>
+  </si>
+  <si>
+    <t>Nariman Point, Mumbai</t>
+  </si>
+  <si>
+    <t>Sayyaji Rao Road, Mysore</t>
+  </si>
+  <si>
+    <t>Station Road, Nagaur</t>
+  </si>
+  <si>
+    <t>Kingsway Road, Nagpur</t>
+  </si>
+  <si>
+    <t>Mall Road, Nainital</t>
+  </si>
+  <si>
+    <t>College Road, Nashik</t>
+  </si>
+  <si>
+    <t>Sector 18, Noida</t>
+  </si>
+  <si>
+    <t>Charing Cross, Ooty</t>
+  </si>
+  <si>
+    <t>MG Road, Panaji</t>
+  </si>
+  <si>
+    <t>Sheranwala Gate, Patiala</t>
+  </si>
+  <si>
+    <t>Fraser Road, Patna</t>
+  </si>
+  <si>
+    <t>Mission Street, Pondicherry</t>
+  </si>
+  <si>
+    <t>Aberdeen Bazaar, Port Blair</t>
+  </si>
+  <si>
+    <t>FC Road, Pune</t>
+  </si>
+  <si>
+    <t>GE Road, Raipur</t>
+  </si>
+  <si>
+    <t>Yagnik Road, Rajkot</t>
+  </si>
+  <si>
+    <t>Main Road, Ranchi</t>
+  </si>
+  <si>
+    <t>Civil Lines, Rohtak</t>
+  </si>
+  <si>
+    <t>Udit Nagar, Rourkela</t>
+  </si>
+  <si>
+    <t>Gugai, Salem</t>
+  </si>
+  <si>
+    <t>Police Bazaar, Shillong</t>
+  </si>
+  <si>
+    <t>Mall Road, Shimla</t>
+  </si>
+  <si>
+    <t>Hill Cart Road, Siliguri</t>
+  </si>
+  <si>
+    <t>Residency Road, Srinagar</t>
+  </si>
+  <si>
+    <t>Ring Road, Surat</t>
+  </si>
+  <si>
+    <t>Ghodbunder Road, Thane</t>
+  </si>
+  <si>
+    <t>MG Road, Thrissur</t>
+  </si>
+  <si>
+    <t>RC Road, Tirupati</t>
+  </si>
+  <si>
+    <t>Cantonment, Trichy</t>
+  </si>
+  <si>
+    <t>City Palace Road, Udaipur</t>
+  </si>
+  <si>
+    <t>Freeganj, Ujjain</t>
+  </si>
+  <si>
+    <t>Raopura, Vadodara</t>
+  </si>
+  <si>
+    <t>Godowlia, Varanasi</t>
+  </si>
+  <si>
+    <t>Katpadi Road, Vellore</t>
+  </si>
+  <si>
+    <t>MG Road, Vijayawada</t>
+  </si>
+  <si>
+    <t>Dwaraka Nagar, Visakhapatnam</t>
+  </si>
+  <si>
     <t>Tripura</t>
   </si>
   <si>
@@ -358,200 +835,77 @@
     <t>Jharkhand</t>
   </si>
   <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
     <t>Kerala</t>
   </si>
   <si>
     <t>Chandigarh</t>
   </si>
   <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
     <t>Uttarakhand</t>
   </si>
   <si>
     <t>Assam</t>
   </si>
   <si>
-    <t>Haryana</t>
-  </si>
-  <si>
-    <t>Andhra Pradesh</t>
-  </si>
-  <si>
-    <t>PPP</t>
-  </si>
-  <si>
-    <t>STATE</t>
-  </si>
-  <si>
-    <t>IFSC_CODE</t>
-  </si>
-  <si>
-    <t>BRANCH_NAME</t>
-  </si>
-  <si>
-    <t>MG Road, Agartala</t>
-  </si>
-  <si>
-    <t>Ashram Road, Ahmedabad</t>
-  </si>
-  <si>
-    <t>Station Road, Akbarpur</t>
-  </si>
-  <si>
-    <t>Civil Lines, Aligarh</t>
-  </si>
-  <si>
-    <t>Alipore Road, Kolkata</t>
-  </si>
-  <si>
-    <t>MG Marg, Allahabad</t>
-  </si>
-  <si>
-    <t>Near Clock Tower, Alwar</t>
-  </si>
-  <si>
-    <t>Main Road, Amravati</t>
-  </si>
-  <si>
-    <t>Golden Temple Road, Amritsar</t>
-  </si>
-  <si>
-    <t>GT Road, Asansol</t>
-  </si>
-  <si>
-    <t>Samarth Nagar, Aurangabad</t>
-  </si>
-  <si>
-    <t>Chandipur Road, Balasore</t>
-  </si>
-  <si>
-    <t>MG Road, Bangalore</t>
-  </si>
-  <si>
-    <t>Civil Lines, Bareilly</t>
-  </si>
-  <si>
-    <t>Gandhi Nagar, Berhampur</t>
-  </si>
-  <si>
-    <t>JLN Road, Bhagalpur</t>
-  </si>
-  <si>
-    <t>Waghawadi Road, Bhavnagar</t>
-  </si>
-  <si>
-    <t>Nehru Nagar, Bhilai</t>
-  </si>
-  <si>
-    <t>TT Nagar, Bhopal</t>
-  </si>
-  <si>
-    <t>Janpath, Bhubaneswar</t>
-  </si>
-  <si>
-    <t>Station Road, Bhuj</t>
-  </si>
-  <si>
-    <t>Link Road, Bilaspur</t>
-  </si>
-  <si>
-    <t>Sector 4, Bokaro</t>
-  </si>
-  <si>
-    <t>G T Road, Burdwan</t>
-  </si>
-  <si>
-    <t>Mavoor Road, Calicut</t>
-  </si>
-  <si>
-    <t>Sector 17, Chandigarh</t>
-  </si>
-  <si>
-    <t>Anna Salai, Chennai</t>
-  </si>
-  <si>
-    <t>Gandhipuram, Coimbatore</t>
-  </si>
-  <si>
-    <t>Buxi Bazar, Cuttack</t>
-  </si>
-  <si>
-    <t>Rajpur Road, Dehradun</t>
-  </si>
-  <si>
-    <t>Bank More, Dhanbad</t>
-  </si>
-  <si>
-    <t>H S Road, Dibrugarh</t>
-  </si>
-  <si>
-    <t>Benachity, Durgapur</t>
-  </si>
-  <si>
-    <t>Marine Drive, Ernakulam</t>
-  </si>
-  <si>
-    <t>Perundurai Road, Erode</t>
-  </si>
-  <si>
-    <t>Sector 15, Faridabad</t>
-  </si>
-  <si>
-    <t>Mall Road, Ferozepur</t>
-  </si>
-  <si>
-    <t>Infocity, Gandhinagar</t>
-  </si>
-  <si>
-    <t>GB Road, Gaya</t>
-  </si>
-  <si>
-    <t>GT Road, Ghaziabad</t>
-  </si>
-  <si>
-    <t>Bank Road, Gorakhpur</t>
-  </si>
-  <si>
-    <t>Arundelpet, Guntur</t>
-  </si>
-  <si>
-    <t>MG Road, Gurgaon</t>
-  </si>
-  <si>
-    <t>Panbazar, Guwahati</t>
-  </si>
-  <si>
-    <t>Lashkar, Gwalior</t>
-  </si>
-  <si>
-    <t>Nainital Road, Haldwani</t>
-  </si>
-  <si>
-    <t>Station Road, Hardoi</t>
-  </si>
-  <si>
-    <t>Near Bus Stand, Hissar</t>
-  </si>
-  <si>
-    <t>Dobson Road, Howrah</t>
-  </si>
-  <si>
-    <t>Lamington Road, Hubli</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>SBIN0000336</t>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>Jammu &amp; Kashmir</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Puducherry</t>
+  </si>
+  <si>
+    <t>Andaman &amp; Nicobar</t>
+  </si>
+  <si>
+    <t>Meghalaya</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>SBIN0070001</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>P12_5</t>
+  </si>
+  <si>
+    <t>P37_5</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>P62_5</t>
+  </si>
+  <si>
+    <t>P75</t>
+  </si>
+  <si>
+    <t>P87_5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,16 +921,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -599,15 +970,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,886 +1305,1782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>258</v>
       </c>
       <c r="E2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="E3">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E4">
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E5">
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="E6">
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="E8">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>263</v>
       </c>
       <c r="E9">
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>264</v>
       </c>
       <c r="E10">
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="E11">
         <v>0.65</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>263</v>
       </c>
       <c r="E12">
         <v>0.65</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>265</v>
       </c>
       <c r="E13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>266</v>
       </c>
       <c r="E14">
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>265</v>
       </c>
       <c r="E16">
         <v>0.45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>267</v>
       </c>
       <c r="E17">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="E18">
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>268</v>
       </c>
       <c r="E19">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>269</v>
       </c>
       <c r="E20">
         <v>0.65</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>265</v>
       </c>
       <c r="E21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="E22">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" t="s">
-        <v>144</v>
-      </c>
-      <c r="D23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E23">
+    <row r="23" spans="1:12" s="6" customFormat="1">
+      <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E23" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="6">
+        <v>2.97</v>
+      </c>
+      <c r="G23" s="6">
+        <v>7.66</v>
+      </c>
+      <c r="H23" s="6">
+        <v>13.17</v>
+      </c>
+      <c r="I23" s="6">
+        <v>21.49</v>
+      </c>
+      <c r="J23" s="6">
+        <v>29</v>
+      </c>
+      <c r="K23" s="6">
+        <v>37.28</v>
+      </c>
+      <c r="L23" s="6">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>270</v>
       </c>
       <c r="E24">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="E25">
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
       <c r="E26">
         <v>0.7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>275</v>
       </c>
       <c r="E27">
         <v>0.85</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>273</v>
       </c>
       <c r="E28">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="D29" t="s">
-        <v>114</v>
+        <v>273</v>
       </c>
       <c r="E29">
         <v>0.75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>265</v>
       </c>
       <c r="E30">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>276</v>
       </c>
       <c r="E31">
         <v>0.65</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>270</v>
       </c>
       <c r="E32">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
       <c r="D33" t="s">
-        <v>116</v>
+        <v>277</v>
       </c>
       <c r="E33">
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="E34">
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
       <c r="E35">
         <v>0.7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
       <c r="D36" t="s">
-        <v>114</v>
+        <v>273</v>
       </c>
       <c r="E36">
         <v>0.75</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>272</v>
       </c>
       <c r="E37">
         <v>0.6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="D38" t="s">
-        <v>105</v>
+        <v>264</v>
       </c>
       <c r="E38">
         <v>0.7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>196</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>259</v>
       </c>
       <c r="E39">
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="D40" t="s">
-        <v>108</v>
+        <v>267</v>
       </c>
       <c r="E40">
         <v>0.75</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E41">
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>199</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E42">
         <v>0.65</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>271</v>
       </c>
       <c r="E43">
         <v>0.85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="D44" t="s">
-        <v>117</v>
+        <v>272</v>
       </c>
       <c r="E44">
         <v>0.7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="D45" t="s">
-        <v>116</v>
+        <v>277</v>
       </c>
       <c r="E45">
         <v>0.6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>203</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>269</v>
       </c>
       <c r="E46">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>276</v>
       </c>
       <c r="E47">
         <v>0.4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>260</v>
       </c>
       <c r="E48">
         <v>0.65</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="D49" t="s">
-        <v>117</v>
+        <v>272</v>
       </c>
       <c r="E49">
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>261</v>
       </c>
       <c r="E50">
         <v>0.7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="C51" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="D51" t="s">
-        <v>107</v>
+        <v>266</v>
       </c>
       <c r="E51">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
+        <v>209</v>
+      </c>
+      <c r="D52" t="s">
+        <v>269</v>
+      </c>
+      <c r="E52">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" t="s">
+        <v>278</v>
+      </c>
+      <c r="E53">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" t="s">
+        <v>269</v>
+      </c>
+      <c r="E54">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" t="s">
+        <v>212</v>
+      </c>
+      <c r="D55" t="s">
+        <v>262</v>
+      </c>
+      <c r="E55">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" t="s">
+        <v>279</v>
+      </c>
+      <c r="E56">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" t="s">
+        <v>214</v>
+      </c>
+      <c r="D57" t="s">
+        <v>270</v>
+      </c>
+      <c r="E57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="s">
+        <v>215</v>
+      </c>
+      <c r="D58" t="s">
+        <v>262</v>
+      </c>
+      <c r="E58">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" t="s">
+        <v>260</v>
+      </c>
+      <c r="E59">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" t="s">
+        <v>274</v>
+      </c>
+      <c r="E60">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>218</v>
+      </c>
+      <c r="D61" t="s">
+        <v>261</v>
+      </c>
+      <c r="E61">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>219</v>
+      </c>
+      <c r="D62" t="s">
+        <v>260</v>
+      </c>
+      <c r="E62">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" t="s">
+        <v>220</v>
+      </c>
+      <c r="D63" t="s">
+        <v>264</v>
+      </c>
+      <c r="E63">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" t="s">
+        <v>221</v>
+      </c>
+      <c r="D64" t="s">
+        <v>273</v>
+      </c>
+      <c r="E64">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="6" customFormat="1">
+      <c r="A65" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E65" s="6">
+        <v>1</v>
+      </c>
+      <c r="F65" s="6">
+        <v>10.71</v>
+      </c>
+      <c r="G65" s="6">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="H65" s="6">
+        <v>54.73</v>
+      </c>
+      <c r="I65" s="6">
+        <v>75.42</v>
+      </c>
+      <c r="J65" s="6">
+        <v>93.99</v>
+      </c>
+      <c r="K65" s="6">
+        <v>100</v>
+      </c>
+      <c r="L65" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" t="s">
+        <v>223</v>
+      </c>
+      <c r="D66" t="s">
+        <v>266</v>
+      </c>
+      <c r="E66">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" t="s">
+        <v>224</v>
+      </c>
+      <c r="D67" t="s">
+        <v>262</v>
+      </c>
+      <c r="E67">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" t="s">
+        <v>225</v>
+      </c>
+      <c r="D68" t="s">
+        <v>263</v>
+      </c>
+      <c r="E68">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>226</v>
+      </c>
+      <c r="D69" t="s">
+        <v>276</v>
+      </c>
+      <c r="E69">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>154</v>
+      </c>
+      <c r="C70" t="s">
+        <v>227</v>
+      </c>
+      <c r="D70" t="s">
+        <v>263</v>
+      </c>
+      <c r="E70">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" t="s">
+        <v>228</v>
+      </c>
+      <c r="D71" t="s">
+        <v>260</v>
+      </c>
+      <c r="E71">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" t="s">
+        <v>229</v>
+      </c>
+      <c r="D72" t="s">
+        <v>273</v>
+      </c>
+      <c r="E72">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" t="s">
+        <v>230</v>
+      </c>
+      <c r="D73" t="s">
+        <v>280</v>
+      </c>
+      <c r="E73">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" t="s">
+        <v>231</v>
+      </c>
+      <c r="D74" t="s">
+        <v>264</v>
+      </c>
+      <c r="E74">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" t="s">
+        <v>232</v>
+      </c>
+      <c r="D75" t="s">
+        <v>267</v>
+      </c>
+      <c r="E75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" t="s">
+        <v>233</v>
+      </c>
+      <c r="D76" t="s">
+        <v>281</v>
+      </c>
+      <c r="E76">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" t="s">
+        <v>234</v>
+      </c>
+      <c r="D77" t="s">
+        <v>282</v>
+      </c>
+      <c r="E77">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" t="s">
+        <v>235</v>
+      </c>
+      <c r="D78" t="s">
+        <v>263</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" t="s">
+        <v>236</v>
+      </c>
+      <c r="D79" t="s">
+        <v>268</v>
+      </c>
+      <c r="E79">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" t="s">
+        <v>237</v>
+      </c>
+      <c r="D80" t="s">
+        <v>259</v>
+      </c>
+      <c r="E80">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" t="s">
+        <v>238</v>
+      </c>
+      <c r="D81" t="s">
+        <v>270</v>
+      </c>
+      <c r="E81">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82" t="s">
+        <v>239</v>
+      </c>
+      <c r="D82" t="s">
+        <v>272</v>
+      </c>
+      <c r="E82">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" t="s">
+        <v>240</v>
+      </c>
+      <c r="D83" t="s">
+        <v>265</v>
+      </c>
+      <c r="E83">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
+        <v>141</v>
+      </c>
+      <c r="C84" t="s">
+        <v>241</v>
+      </c>
+      <c r="D84" t="s">
+        <v>273</v>
+      </c>
+      <c r="E84">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" t="s">
+        <v>142</v>
+      </c>
+      <c r="C85" t="s">
+        <v>242</v>
+      </c>
+      <c r="D85" t="s">
+        <v>283</v>
+      </c>
+      <c r="E85">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>143</v>
+      </c>
+      <c r="C86" t="s">
+        <v>243</v>
+      </c>
+      <c r="D86" t="s">
+        <v>284</v>
+      </c>
+      <c r="E86">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" t="s">
+        <v>244</v>
+      </c>
+      <c r="D87" t="s">
+        <v>261</v>
+      </c>
+      <c r="E87">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
+        <v>145</v>
+      </c>
+      <c r="C88" t="s">
+        <v>245</v>
+      </c>
+      <c r="D88" t="s">
+        <v>279</v>
+      </c>
+      <c r="E88">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" t="s">
+        <v>146</v>
+      </c>
+      <c r="C89" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" t="s">
+        <v>259</v>
+      </c>
+      <c r="E89">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90" t="s">
+        <v>247</v>
+      </c>
+      <c r="D90" t="s">
+        <v>263</v>
+      </c>
+      <c r="E90">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" t="s">
+        <v>148</v>
+      </c>
+      <c r="C91" t="s">
+        <v>248</v>
+      </c>
+      <c r="D91" t="s">
+        <v>274</v>
+      </c>
+      <c r="E91">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s">
+        <v>149</v>
+      </c>
+      <c r="C92" t="s">
+        <v>249</v>
+      </c>
+      <c r="D92" t="s">
+        <v>271</v>
+      </c>
+      <c r="E92">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="s">
+        <v>150</v>
+      </c>
+      <c r="C93" t="s">
+        <v>250</v>
+      </c>
+      <c r="D93" t="s">
+        <v>273</v>
+      </c>
+      <c r="E93">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="s">
+        <v>151</v>
+      </c>
+      <c r="C94" t="s">
+        <v>251</v>
+      </c>
+      <c r="D94" t="s">
+        <v>262</v>
+      </c>
+      <c r="E94">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="s">
+        <v>152</v>
+      </c>
+      <c r="C95" t="s">
+        <v>252</v>
+      </c>
+      <c r="D95" t="s">
+        <v>269</v>
+      </c>
+      <c r="E95">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96" t="s">
+        <v>153</v>
+      </c>
+      <c r="C96" t="s">
+        <v>253</v>
+      </c>
+      <c r="D96" t="s">
+        <v>259</v>
+      </c>
+      <c r="E96">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" t="s">
+        <v>254</v>
+      </c>
+      <c r="D97" t="s">
+        <v>260</v>
+      </c>
+      <c r="E97">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98" t="s">
+        <v>156</v>
+      </c>
+      <c r="C98" t="s">
+        <v>255</v>
+      </c>
+      <c r="D98" t="s">
+        <v>273</v>
+      </c>
+      <c r="E98">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99" t="s">
+        <v>157</v>
+      </c>
+      <c r="C99" t="s">
+        <v>256</v>
+      </c>
+      <c r="D99" t="s">
+        <v>271</v>
+      </c>
+      <c r="E99">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100" t="s">
+        <v>257</v>
+      </c>
+      <c r="D100" t="s">
+        <v>271</v>
+      </c>
+      <c r="E100">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: persona.py, proper output formatting, many minor and major fixes
</commit_message>
<xml_diff>
--- a/data/branch.xlsx
+++ b/data/branch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Surojit Mondal\Desktop\sbi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE85129-8CA5-48CE-A337-2546D6B5C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C27BA55-CC45-4F94-A8B8-7EC0F960CF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,27 @@
     <t>PPP</t>
   </si>
   <si>
+    <t>P12_5</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>P37_5</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>P62_5</t>
+  </si>
+  <si>
+    <t>P75</t>
+  </si>
+  <si>
+    <t>P87_5</t>
+  </si>
+  <si>
     <t>Agartala</t>
   </si>
   <si>
@@ -484,6 +505,9 @@
     <t>SBIN0000050</t>
   </si>
   <si>
+    <t>SBIN0070001</t>
+  </si>
+  <si>
     <t>SBIN0000022</t>
   </si>
   <si>
@@ -835,27 +859,27 @@
     <t>Jharkhand</t>
   </si>
   <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Uttarakhand</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
     <t>Andhra Pradesh</t>
   </si>
   <si>
-    <t>Haryana</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
-    <t>Kerala</t>
-  </si>
-  <si>
-    <t>Chandigarh</t>
-  </si>
-  <si>
-    <t>Uttarakhand</t>
-  </si>
-  <si>
-    <t>Assam</t>
-  </si>
-  <si>
     <t>Arunachal Pradesh</t>
   </si>
   <si>
@@ -875,37 +899,13 @@
   </si>
   <si>
     <t>Himachal Pradesh</t>
-  </si>
-  <si>
-    <t>SBIN0070001</t>
-  </si>
-  <si>
-    <t>P25</t>
-  </si>
-  <si>
-    <t>P12_5</t>
-  </si>
-  <si>
-    <t>P37_5</t>
-  </si>
-  <si>
-    <t>P50</t>
-  </si>
-  <si>
-    <t>P62_5</t>
-  </si>
-  <si>
-    <t>P75</t>
-  </si>
-  <si>
-    <t>P87_5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -921,33 +921,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -970,37 +953,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,19 +1268,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1335,1752 +1296,3788 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="E2">
         <v>0.5</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="F2">
+        <v>2.97</v>
+      </c>
+      <c r="G2">
+        <v>7.66</v>
+      </c>
+      <c r="H2">
+        <v>13.17</v>
+      </c>
+      <c r="I2">
+        <v>21.49</v>
+      </c>
+      <c r="J2">
+        <v>29</v>
+      </c>
+      <c r="K2">
+        <v>37.28</v>
+      </c>
+      <c r="L2">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E3">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="F3">
+        <v>8.8524000000000012</v>
+      </c>
+      <c r="G3">
+        <v>28.7804</v>
+      </c>
+      <c r="H3">
+        <v>44.755599999999987</v>
+      </c>
+      <c r="I3">
+        <v>62.476799999999997</v>
+      </c>
+      <c r="J3">
+        <v>78.392399999999995</v>
+      </c>
+      <c r="K3">
+        <v>84.947200000000009</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="F4">
+        <v>1.422000000000001</v>
+      </c>
+      <c r="G4">
+        <v>2.1020000000000012</v>
+      </c>
+      <c r="H4">
+        <v>4.8580000000000023</v>
+      </c>
+      <c r="I4">
+        <v>10.704000000000001</v>
+      </c>
+      <c r="J4">
+        <v>16.001999999999999</v>
+      </c>
+      <c r="K4">
+        <v>24.736000000000001</v>
+      </c>
+      <c r="L4">
+        <v>42.58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E5">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="F5">
+        <v>2.1960000000000011</v>
+      </c>
+      <c r="G5">
+        <v>4.8810000000000002</v>
+      </c>
+      <c r="H5">
+        <v>9.0140000000000011</v>
+      </c>
+      <c r="I5">
+        <v>16.097000000000001</v>
+      </c>
+      <c r="J5">
+        <v>22.501000000000001</v>
+      </c>
+      <c r="K5">
+        <v>31.007999999999999</v>
+      </c>
+      <c r="L5">
+        <v>47.365000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E6">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="F6">
+        <v>8.3879999999999999</v>
+      </c>
+      <c r="G6">
+        <v>27.113</v>
+      </c>
+      <c r="H6">
+        <v>42.261999999999993</v>
+      </c>
+      <c r="I6">
+        <v>59.241</v>
+      </c>
+      <c r="J6">
+        <v>74.492999999999995</v>
+      </c>
+      <c r="K6">
+        <v>81.183999999999997</v>
+      </c>
+      <c r="L6">
+        <v>85.644999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="F7">
+        <v>2.97</v>
+      </c>
+      <c r="G7">
+        <v>7.66</v>
+      </c>
+      <c r="H7">
+        <v>13.17</v>
+      </c>
+      <c r="I7">
+        <v>21.49</v>
+      </c>
+      <c r="J7">
+        <v>29</v>
+      </c>
+      <c r="K7">
+        <v>37.28</v>
+      </c>
+      <c r="L7">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E8">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="F8">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G8">
+        <v>10.439</v>
+      </c>
+      <c r="H8">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I8">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J8">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K8">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L8">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="F9">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G9">
+        <v>13.218</v>
+      </c>
+      <c r="H9">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I9">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J9">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K9">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L9">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E10">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="F10">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G10">
+        <v>18.776</v>
+      </c>
+      <c r="H10">
+        <v>29.794</v>
+      </c>
+      <c r="I10">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J10">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K10">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L10">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E11">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="F11">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G11">
+        <v>15.997</v>
+      </c>
+      <c r="H11">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I11">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J11">
+        <v>48.497</v>
+      </c>
+      <c r="K11">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L11">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E12">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="F12">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G12">
+        <v>15.997</v>
+      </c>
+      <c r="H12">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I12">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J12">
+        <v>48.497</v>
+      </c>
+      <c r="K12">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L12">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D13" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="F13">
+        <v>2.97</v>
+      </c>
+      <c r="G13">
+        <v>7.66</v>
+      </c>
+      <c r="H13">
+        <v>13.17</v>
+      </c>
+      <c r="I13">
+        <v>21.49</v>
+      </c>
+      <c r="J13">
+        <v>29</v>
+      </c>
+      <c r="K13">
+        <v>37.28</v>
+      </c>
+      <c r="L13">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D14" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E14">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>1.95</v>
+      </c>
+      <c r="F14">
+        <v>19.161999999999999</v>
+      </c>
+      <c r="G14">
+        <v>35.892000000000003</v>
+      </c>
+      <c r="H14">
+        <v>56.417999999999999</v>
+      </c>
+      <c r="I14">
+        <v>75.634</v>
+      </c>
+      <c r="J14">
+        <v>90.992000000000004</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E15">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="F15">
+        <v>2.97</v>
+      </c>
+      <c r="G15">
+        <v>7.66</v>
+      </c>
+      <c r="H15">
+        <v>13.17</v>
+      </c>
+      <c r="I15">
+        <v>21.49</v>
+      </c>
+      <c r="J15">
+        <v>29</v>
+      </c>
+      <c r="K15">
+        <v>37.28</v>
+      </c>
+      <c r="L15">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D16" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E16">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="F16">
+        <v>2.1960000000000011</v>
+      </c>
+      <c r="G16">
+        <v>4.8810000000000002</v>
+      </c>
+      <c r="H16">
+        <v>9.0140000000000011</v>
+      </c>
+      <c r="I16">
+        <v>16.097000000000001</v>
+      </c>
+      <c r="J16">
+        <v>22.501000000000001</v>
+      </c>
+      <c r="K16">
+        <v>31.007999999999999</v>
+      </c>
+      <c r="L16">
+        <v>47.365000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E17">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="F17">
+        <v>1.422000000000001</v>
+      </c>
+      <c r="G17">
+        <v>2.1020000000000012</v>
+      </c>
+      <c r="H17">
+        <v>4.8580000000000023</v>
+      </c>
+      <c r="I17">
+        <v>10.704000000000001</v>
+      </c>
+      <c r="J17">
+        <v>16.001999999999999</v>
+      </c>
+      <c r="K17">
+        <v>24.736000000000001</v>
+      </c>
+      <c r="L17">
+        <v>42.58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D18" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E18">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="F18">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G18">
+        <v>13.218</v>
+      </c>
+      <c r="H18">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I18">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J18">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K18">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L18">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C19" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="E19">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="F19">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G19">
+        <v>10.439</v>
+      </c>
+      <c r="H19">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I19">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J19">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K19">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L19">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C20" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D20" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E20">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="F20">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G20">
+        <v>15.997</v>
+      </c>
+      <c r="H20">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I20">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J20">
+        <v>48.497</v>
+      </c>
+      <c r="K20">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L20">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D21" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E21">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="F21">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G21">
+        <v>13.218</v>
+      </c>
+      <c r="H21">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I21">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J21">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K21">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L21">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D22" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E22">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" s="6" customFormat="1">
-      <c r="A23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="E23" s="6">
+      <c r="F22">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G22">
+        <v>10.439</v>
+      </c>
+      <c r="H22">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I22">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J22">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K22">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L22">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D23" t="s">
+        <v>276</v>
+      </c>
+      <c r="E23">
         <v>0.5</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23">
         <v>2.97</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23">
         <v>7.66</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23">
         <v>13.17</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23">
         <v>21.49</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23">
         <v>29</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23">
         <v>37.28</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23">
         <v>52.15</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D24" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="E24">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="F24">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G24">
+        <v>10.439</v>
+      </c>
+      <c r="H24">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I24">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J24">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K24">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L24">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D25" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E25">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="F25">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G25">
+        <v>13.218</v>
+      </c>
+      <c r="H25">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I25">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J25">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K25">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L25">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D26" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E26">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="F26">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G26">
+        <v>18.776</v>
+      </c>
+      <c r="H26">
+        <v>29.794</v>
+      </c>
+      <c r="I26">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J26">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K26">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L26">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D27" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="E27">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="F27">
+        <v>8.3879999999999999</v>
+      </c>
+      <c r="G27">
+        <v>27.113</v>
+      </c>
+      <c r="H27">
+        <v>42.261999999999993</v>
+      </c>
+      <c r="I27">
+        <v>59.241</v>
+      </c>
+      <c r="J27">
+        <v>74.492999999999995</v>
+      </c>
+      <c r="K27">
+        <v>81.183999999999997</v>
+      </c>
+      <c r="L27">
+        <v>95.644999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D28" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E28">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="F28">
+        <v>10.400399999999999</v>
+      </c>
+      <c r="G28">
+        <v>34.3384</v>
+      </c>
+      <c r="H28">
+        <v>53.067599999999999</v>
+      </c>
+      <c r="I28">
+        <v>73.262799999999999</v>
+      </c>
+      <c r="J28">
+        <v>91.3904</v>
+      </c>
+      <c r="K28">
+        <v>100</v>
+      </c>
+      <c r="L28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D29" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E29">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="F29">
+        <v>6.84</v>
+      </c>
+      <c r="G29">
+        <v>21.555</v>
+      </c>
+      <c r="H29">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I29">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J29">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K29">
+        <v>68.64</v>
+      </c>
+      <c r="L29">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E30">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="F30">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G30">
+        <v>10.439</v>
+      </c>
+      <c r="H30">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I30">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J30">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K30">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L30">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D31" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E31">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="F31">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G31">
+        <v>15.997</v>
+      </c>
+      <c r="H31">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I31">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J31">
+        <v>48.497</v>
+      </c>
+      <c r="K31">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L31">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D32" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="E32">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G32">
+        <v>10.439</v>
+      </c>
+      <c r="H32">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I32">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J32">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K32">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L32">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D33" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E33">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G33">
+        <v>13.218</v>
+      </c>
+      <c r="H33">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I33">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J33">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K33">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L33">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="D34" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E34">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <v>6.84</v>
+      </c>
+      <c r="G34">
+        <v>21.555</v>
+      </c>
+      <c r="H34">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I34">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J34">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K34">
+        <v>68.64</v>
+      </c>
+      <c r="L34">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D35" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E35">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G35">
+        <v>18.776</v>
+      </c>
+      <c r="H35">
+        <v>29.794</v>
+      </c>
+      <c r="I35">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J35">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K35">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L35">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C36" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D36" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E36">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <v>6.84</v>
+      </c>
+      <c r="G36">
+        <v>21.555</v>
+      </c>
+      <c r="H36">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I36">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J36">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K36">
+        <v>68.64</v>
+      </c>
+      <c r="L36">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D37" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="E37">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G37">
+        <v>13.218</v>
+      </c>
+      <c r="H37">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I37">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J37">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K37">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L37">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="D38" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E38">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G38">
+        <v>18.776</v>
+      </c>
+      <c r="H38">
+        <v>29.794</v>
+      </c>
+      <c r="I38">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J38">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K38">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L38">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D39" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E39">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <v>7.6140000000000008</v>
+      </c>
+      <c r="G39">
+        <v>24.334</v>
+      </c>
+      <c r="H39">
+        <v>38.106000000000002</v>
+      </c>
+      <c r="I39">
+        <v>53.848000000000013</v>
+      </c>
+      <c r="J39">
+        <v>67.994</v>
+      </c>
+      <c r="K39">
+        <v>74.912000000000006</v>
+      </c>
+      <c r="L39">
+        <v>80.86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D40" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E40">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <v>6.84</v>
+      </c>
+      <c r="G40">
+        <v>21.555</v>
+      </c>
+      <c r="H40">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I40">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J40">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K40">
+        <v>68.64</v>
+      </c>
+      <c r="L40">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D41" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E41">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <v>2.97</v>
+      </c>
+      <c r="G41">
+        <v>7.66</v>
+      </c>
+      <c r="H41">
+        <v>13.17</v>
+      </c>
+      <c r="I41">
+        <v>21.49</v>
+      </c>
+      <c r="J41">
+        <v>29</v>
+      </c>
+      <c r="K41">
+        <v>37.28</v>
+      </c>
+      <c r="L41">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C42" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="D42" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E42">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G42">
+        <v>15.997</v>
+      </c>
+      <c r="H42">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I42">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J42">
+        <v>48.497</v>
+      </c>
+      <c r="K42">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L42">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C43" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D43" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="E43">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <v>8.3879999999999999</v>
+      </c>
+      <c r="G43">
+        <v>27.113</v>
+      </c>
+      <c r="H43">
+        <v>42.261999999999993</v>
+      </c>
+      <c r="I43">
+        <v>59.241</v>
+      </c>
+      <c r="J43">
+        <v>74.492999999999995</v>
+      </c>
+      <c r="K43">
+        <v>81.183999999999997</v>
+      </c>
+      <c r="L43">
+        <v>85.644999999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D44" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="E44">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G44">
+        <v>18.776</v>
+      </c>
+      <c r="H44">
+        <v>29.794</v>
+      </c>
+      <c r="I44">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J44">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K44">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L44">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C45" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E45">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G45">
+        <v>13.218</v>
+      </c>
+      <c r="H45">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I45">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J45">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K45">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L45">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D46" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E46">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G46">
+        <v>10.439</v>
+      </c>
+      <c r="H46">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I46">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J46">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K46">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L46">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D47" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E47">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <v>1.422000000000001</v>
+      </c>
+      <c r="G47">
+        <v>2.1020000000000012</v>
+      </c>
+      <c r="H47">
+        <v>4.8580000000000023</v>
+      </c>
+      <c r="I47">
+        <v>10.704000000000001</v>
+      </c>
+      <c r="J47">
+        <v>16.001999999999999</v>
+      </c>
+      <c r="K47">
+        <v>24.736000000000001</v>
+      </c>
+      <c r="L47">
+        <v>42.58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D48" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E48">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G48">
+        <v>15.997</v>
+      </c>
+      <c r="H48">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I48">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J48">
+        <v>48.497</v>
+      </c>
+      <c r="K48">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L48">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="D49" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="E49">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <v>6.84</v>
+      </c>
+      <c r="G49">
+        <v>21.555</v>
+      </c>
+      <c r="H49">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I49">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J49">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K49">
+        <v>68.64</v>
+      </c>
+      <c r="L49">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D50" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E50">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G50">
+        <v>18.776</v>
+      </c>
+      <c r="H50">
+        <v>29.794</v>
+      </c>
+      <c r="I50">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J50">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K50">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L50">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C51" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D51" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E51">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <v>7.6140000000000008</v>
+      </c>
+      <c r="G51">
+        <v>24.334</v>
+      </c>
+      <c r="H51">
+        <v>38.106000000000002</v>
+      </c>
+      <c r="I51">
+        <v>53.848000000000013</v>
+      </c>
+      <c r="J51">
+        <v>67.994</v>
+      </c>
+      <c r="K51">
+        <v>74.912000000000006</v>
+      </c>
+      <c r="L51">
+        <v>80.86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D52" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E52">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G52">
+        <v>18.776</v>
+      </c>
+      <c r="H52">
+        <v>29.794</v>
+      </c>
+      <c r="I52">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J52">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K52">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L52">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="D53" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="E53">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <v>1.422000000000001</v>
+      </c>
+      <c r="G53">
+        <v>2.1020000000000012</v>
+      </c>
+      <c r="H53">
+        <v>4.8580000000000023</v>
+      </c>
+      <c r="I53">
+        <v>10.704000000000001</v>
+      </c>
+      <c r="J53">
+        <v>16.001999999999999</v>
+      </c>
+      <c r="K53">
+        <v>24.736000000000001</v>
+      </c>
+      <c r="L53">
+        <v>42.58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D54" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E54">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G54">
+        <v>13.218</v>
+      </c>
+      <c r="H54">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I54">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J54">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K54">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L54">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="D55" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E55">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <v>6.84</v>
+      </c>
+      <c r="G55">
+        <v>21.555</v>
+      </c>
+      <c r="H55">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I55">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J55">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K55">
+        <v>68.64</v>
+      </c>
+      <c r="L55">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="D56" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="E56">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G56">
+        <v>10.439</v>
+      </c>
+      <c r="H56">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I56">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J56">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K56">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L56">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D57" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="E57">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <v>2.97</v>
+      </c>
+      <c r="G57">
+        <v>7.66</v>
+      </c>
+      <c r="H57">
+        <v>13.17</v>
+      </c>
+      <c r="I57">
+        <v>21.49</v>
+      </c>
+      <c r="J57">
+        <v>29</v>
+      </c>
+      <c r="K57">
+        <v>37.28</v>
+      </c>
+      <c r="L57">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C58" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D58" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E58">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G58">
+        <v>15.997</v>
+      </c>
+      <c r="H58">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I58">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J58">
+        <v>48.497</v>
+      </c>
+      <c r="K58">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L58">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D59" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E59">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G59">
+        <v>10.439</v>
+      </c>
+      <c r="H59">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I59">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J59">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K59">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L59">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="D60" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E60">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <v>7.6140000000000008</v>
+      </c>
+      <c r="G60">
+        <v>24.334</v>
+      </c>
+      <c r="H60">
+        <v>38.106000000000002</v>
+      </c>
+      <c r="I60">
+        <v>53.848000000000013</v>
+      </c>
+      <c r="J60">
+        <v>67.994</v>
+      </c>
+      <c r="K60">
+        <v>74.912000000000006</v>
+      </c>
+      <c r="L60">
+        <v>80.86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C61" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D61" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E61">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61">
+        <v>8.8524000000000012</v>
+      </c>
+      <c r="G61">
+        <v>28.7804</v>
+      </c>
+      <c r="H61">
+        <v>44.755599999999987</v>
+      </c>
+      <c r="I61">
+        <v>62.476799999999997</v>
+      </c>
+      <c r="J61">
+        <v>78.392399999999995</v>
+      </c>
+      <c r="K61">
+        <v>84.947200000000009</v>
+      </c>
+      <c r="L61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="D62" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E62">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G62">
+        <v>13.218</v>
+      </c>
+      <c r="H62">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I62">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J62">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K62">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L62">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D63" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E63">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G63">
+        <v>15.997</v>
+      </c>
+      <c r="H63">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I63">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J63">
+        <v>48.497</v>
+      </c>
+      <c r="K63">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L63">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D64" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E64">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" s="6" customFormat="1">
-      <c r="A65" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="E65" s="6">
+      <c r="F64">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G64">
+        <v>10.439</v>
+      </c>
+      <c r="H64">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I64">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J64">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K64">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L64">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" t="s">
+        <v>230</v>
+      </c>
+      <c r="D65" t="s">
+        <v>271</v>
+      </c>
+      <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65" s="6">
+      <c r="F65">
         <v>10.71</v>
       </c>
-      <c r="G65" s="6">
+      <c r="G65">
         <v>35.450000000000003</v>
       </c>
-      <c r="H65" s="6">
+      <c r="H65">
         <v>54.73</v>
       </c>
-      <c r="I65" s="6">
+      <c r="I65">
         <v>75.42</v>
       </c>
-      <c r="J65" s="6">
+      <c r="J65">
         <v>93.99</v>
       </c>
-      <c r="K65" s="6">
+      <c r="K65">
         <v>100</v>
       </c>
-      <c r="L65" s="6">
+      <c r="L65">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C66" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D66" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E66">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="F66">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G66">
+        <v>13.218</v>
+      </c>
+      <c r="H66">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I66">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J66">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K66">
+        <v>69.823999999999998</v>
+      </c>
+      <c r="L66">
+        <v>81.72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C67" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D67" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E67">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="F67">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G67">
+        <v>10.439</v>
+      </c>
+      <c r="H67">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I67">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J67">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K67">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L67">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C68" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D68" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E68">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="F68">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G68">
+        <v>15.997</v>
+      </c>
+      <c r="H68">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I68">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J68">
+        <v>48.497</v>
+      </c>
+      <c r="K68">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L68">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="D69" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E69">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="F69">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G69">
+        <v>13.218</v>
+      </c>
+      <c r="H69">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I69">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J69">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K69">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L69">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C70" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="D70" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E70">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="F70">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G70">
+        <v>13.218</v>
+      </c>
+      <c r="H70">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I70">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J70">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K70">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L70">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="D71" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E71">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="F71">
+        <v>6.84</v>
+      </c>
+      <c r="G71">
+        <v>21.555</v>
+      </c>
+      <c r="H71">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I71">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J71">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K71">
+        <v>68.64</v>
+      </c>
+      <c r="L71">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C72" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="D72" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E72">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="F72">
+        <v>2.97</v>
+      </c>
+      <c r="G72">
+        <v>7.66</v>
+      </c>
+      <c r="H72">
+        <v>13.17</v>
+      </c>
+      <c r="I72">
+        <v>21.49</v>
+      </c>
+      <c r="J72">
+        <v>29</v>
+      </c>
+      <c r="K72">
+        <v>37.28</v>
+      </c>
+      <c r="L72">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C73" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="D73" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="E73">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="F73">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G73">
+        <v>18.776</v>
+      </c>
+      <c r="H73">
+        <v>29.794</v>
+      </c>
+      <c r="I73">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J73">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K73">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L73">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C74" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="D74" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E74">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="F74">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G74">
+        <v>15.997</v>
+      </c>
+      <c r="H74">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I74">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J74">
+        <v>48.497</v>
+      </c>
+      <c r="K74">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L74">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C75" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D75" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E75">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="F75">
+        <v>2.97</v>
+      </c>
+      <c r="G75">
+        <v>7.66</v>
+      </c>
+      <c r="H75">
+        <v>13.17</v>
+      </c>
+      <c r="I75">
+        <v>21.49</v>
+      </c>
+      <c r="J75">
+        <v>29</v>
+      </c>
+      <c r="K75">
+        <v>37.28</v>
+      </c>
+      <c r="L75">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C76" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="D76" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="E76">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="F76">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G76">
+        <v>13.218</v>
+      </c>
+      <c r="H76">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I76">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J76">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K76">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L76">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="D77" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="E77">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="F77">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G77">
+        <v>10.439</v>
+      </c>
+      <c r="H77">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I77">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J77">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K77">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L77">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C78" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="D78" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="F78">
+        <v>10.71</v>
+      </c>
+      <c r="G78">
+        <v>35.450000000000003</v>
+      </c>
+      <c r="H78">
+        <v>54.73</v>
+      </c>
+      <c r="I78">
+        <v>75.42</v>
+      </c>
+      <c r="J78">
+        <v>93.99</v>
+      </c>
+      <c r="K78">
+        <v>100</v>
+      </c>
+      <c r="L78">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C79" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D79" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="E79">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="F79">
+        <v>2.97</v>
+      </c>
+      <c r="G79">
+        <v>7.66</v>
+      </c>
+      <c r="H79">
+        <v>13.17</v>
+      </c>
+      <c r="I79">
+        <v>21.49</v>
+      </c>
+      <c r="J79">
+        <v>29</v>
+      </c>
+      <c r="K79">
+        <v>37.28</v>
+      </c>
+      <c r="L79">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="D80" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E80">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G80">
+        <v>18.776</v>
+      </c>
+      <c r="H80">
+        <v>29.794</v>
+      </c>
+      <c r="I80">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J80">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K80">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L80">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="D81" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="E81">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G81">
+        <v>10.439</v>
+      </c>
+      <c r="H81">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I81">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J81">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K81">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L81">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C82" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D82" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="E82">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <v>2.97</v>
+      </c>
+      <c r="G82">
+        <v>7.66</v>
+      </c>
+      <c r="H82">
+        <v>13.17</v>
+      </c>
+      <c r="I82">
+        <v>21.49</v>
+      </c>
+      <c r="J82">
+        <v>29</v>
+      </c>
+      <c r="K82">
+        <v>37.28</v>
+      </c>
+      <c r="L82">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C83" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E83">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <v>2.97</v>
+      </c>
+      <c r="G83">
+        <v>7.66</v>
+      </c>
+      <c r="H83">
+        <v>13.17</v>
+      </c>
+      <c r="I83">
+        <v>21.49</v>
+      </c>
+      <c r="J83">
+        <v>29</v>
+      </c>
+      <c r="K83">
+        <v>37.28</v>
+      </c>
+      <c r="L83">
+        <v>52.15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B84" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C84" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D84" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E84">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G84">
+        <v>10.439</v>
+      </c>
+      <c r="H84">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I84">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J84">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K84">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L84">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C85" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="D85" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="E85">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <v>2.1960000000000011</v>
+      </c>
+      <c r="G85">
+        <v>4.8810000000000002</v>
+      </c>
+      <c r="H85">
+        <v>9.0140000000000011</v>
+      </c>
+      <c r="I85">
+        <v>16.097000000000001</v>
+      </c>
+      <c r="J85">
+        <v>22.501000000000001</v>
+      </c>
+      <c r="K85">
+        <v>31.007999999999999</v>
+      </c>
+      <c r="L85">
+        <v>47.365000000000002</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="D86" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E86">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G86">
+        <v>15.997</v>
+      </c>
+      <c r="H86">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I86">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J86">
+        <v>48.497</v>
+      </c>
+      <c r="K86">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L86">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C87" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D87" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="E87">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G87">
+        <v>13.218</v>
+      </c>
+      <c r="H87">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I87">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J87">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K87">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L87">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B88" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C88" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="D88" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="E88">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G88">
+        <v>10.439</v>
+      </c>
+      <c r="H88">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I88">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J88">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K88">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L88">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C89" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="D89" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E89">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <v>6.84</v>
+      </c>
+      <c r="G89">
+        <v>21.555</v>
+      </c>
+      <c r="H89">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="I89">
+        <v>48.454999999999998</v>
+      </c>
+      <c r="J89">
+        <v>61.494999999999997</v>
+      </c>
+      <c r="K89">
+        <v>68.64</v>
+      </c>
+      <c r="L89">
+        <v>76.075000000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B90" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C90" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="D90" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="E90">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <v>7.6140000000000008</v>
+      </c>
+      <c r="G90">
+        <v>24.334</v>
+      </c>
+      <c r="H90">
+        <v>38.106000000000002</v>
+      </c>
+      <c r="I90">
+        <v>53.848000000000013</v>
+      </c>
+      <c r="J90">
+        <v>72.994</v>
+      </c>
+      <c r="K90">
+        <v>84.912000000000006</v>
+      </c>
+      <c r="L90">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C91" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="D91" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E91">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G91">
+        <v>15.997</v>
+      </c>
+      <c r="H91">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I91">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J91">
+        <v>48.497</v>
+      </c>
+      <c r="K91">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L91">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C92" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="D92" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="E92">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G92">
+        <v>10.439</v>
+      </c>
+      <c r="H92">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I92">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J92">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K92">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L92">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C93" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="D93" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E93">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G93">
+        <v>13.218</v>
+      </c>
+      <c r="H93">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I93">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J93">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K93">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L93">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C94" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="D94" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="E94">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G94">
+        <v>15.997</v>
+      </c>
+      <c r="H94">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I94">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J94">
+        <v>48.497</v>
+      </c>
+      <c r="K94">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L94">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C95" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="D95" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E95">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G95">
+        <v>10.439</v>
+      </c>
+      <c r="H95">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I95">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J95">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K95">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L95">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B96" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C96" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="D96" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="E96">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G96">
+        <v>18.776</v>
+      </c>
+      <c r="H96">
+        <v>29.794</v>
+      </c>
+      <c r="I96">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J96">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K96">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L96">
+        <v>71.289999999999992</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B97" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C97" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D97" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="E97">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97">
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G97">
+        <v>13.218</v>
+      </c>
+      <c r="H97">
+        <v>21.481999999999999</v>
+      </c>
+      <c r="I97">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="J97">
+        <v>41.997999999999998</v>
+      </c>
+      <c r="K97">
+        <v>49.823999999999998</v>
+      </c>
+      <c r="L97">
+        <v>61.72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B98" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C98" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D98" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="E98">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98">
+        <v>3.7440000000000011</v>
+      </c>
+      <c r="G98">
+        <v>10.439</v>
+      </c>
+      <c r="H98">
+        <v>17.326000000000001</v>
+      </c>
+      <c r="I98">
+        <v>26.882999999999999</v>
+      </c>
+      <c r="J98">
+        <v>35.499000000000002</v>
+      </c>
+      <c r="K98">
+        <v>43.552000000000007</v>
+      </c>
+      <c r="L98">
+        <v>56.935000000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="C99" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D99" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="E99">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99">
+        <v>5.2920000000000007</v>
+      </c>
+      <c r="G99">
+        <v>15.997</v>
+      </c>
+      <c r="H99">
+        <v>25.638000000000002</v>
+      </c>
+      <c r="I99">
+        <v>37.668999999999997</v>
+      </c>
+      <c r="J99">
+        <v>48.497</v>
+      </c>
+      <c r="K99">
+        <v>56.095999999999997</v>
+      </c>
+      <c r="L99">
+        <v>66.504999999999995</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B100" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C100" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="D100" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="E100">
         <v>0.7</v>
+      </c>
+      <c r="F100">
+        <v>6.0659999999999989</v>
+      </c>
+      <c r="G100">
+        <v>18.776</v>
+      </c>
+      <c r="H100">
+        <v>29.794</v>
+      </c>
+      <c r="I100">
+        <v>43.061999999999998</v>
+      </c>
+      <c r="J100">
+        <v>54.996000000000002</v>
+      </c>
+      <c r="K100">
+        <v>62.367999999999988</v>
+      </c>
+      <c r="L100">
+        <v>71.289999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>